<commit_message>
Adição dos arquivos do trabalho 2
</commit_message>
<xml_diff>
--- a/Analise Git e Base de Dados.xlsx
+++ b/Analise Git e Base de Dados.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Desktop\Analise Git\AnaliseGIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC777085-3FCD-4A9B-A934-87391A83843A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16620" windowHeight="9810" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Recolhidos" sheetId="1" r:id="rId1"/>
@@ -18,10 +19,10 @@
     <sheet name="Analise Fase II" sheetId="4" r:id="rId4"/>
     <sheet name="Base de Dados Analise II" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="5" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="121">
   <si>
     <t>files</t>
   </si>
@@ -649,12 +650,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,8 +684,16 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -703,8 +712,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -903,13 +918,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -929,6 +953,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -959,32 +987,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
     <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
-  <dxfs count="53">
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1137,13 +1147,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1153,6 +1156,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1190,6 +1200,12 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -1379,7 +1395,7 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -1394,7 +1410,7 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -1403,7 +1419,7 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -1418,7 +1434,7 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -1427,7 +1443,7 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -1442,7 +1458,7 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -1479,7 +1495,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1793,7 +1808,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1895,7 +1909,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2021,7 +2034,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2059,9 +2071,7 @@
           <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -3029,9 +3039,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3139,7 +3147,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3241,7 +3248,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3884,7 +3890,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3964,6 +3969,377 @@
       </c16:pivotOptions16>
     </c:ext>
   </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cobertura</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de documentação por repositorio</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.8682065965530534E-2"/>
+          <c:y val="8.4319401376160341E-2"/>
+          <c:w val="0.93849742121395663"/>
+          <c:h val="0.76291387693677482"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Analise Fase II'!$I$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cobertura de Documentacao</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Analise Fase II'!$H$25:$H$34</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Tensorflow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>React Native</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>VsCode</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Font Awesome</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Moby</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Angular</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ansible</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Angular Cli</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Cli</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>PatchWork</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Analise Fase II'!$I$25:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.24363401708656748</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21537365808782616</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3243474265687937E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6421496636959249E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13564887718780244</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17494828164837531</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45140451282899458</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14252952959867377</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10359961395621579</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9627791563275434E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4439-467C-BA1C-7579965E1DC5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="459691472"/>
+        <c:axId val="458333072"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="459691472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="458333072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="458333072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="459691472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -4048,6 +4424,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5597,6 +6013,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -5614,7 +6533,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5657,7 +6582,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5687,7 +6618,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 4"/>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5717,7 +6654,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5735,8 +6678,151 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C2D07A6-2110-4679-B69F-47CB13401BBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector de Seta Reta 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7480D968-C13F-41AB-AC1F-9AC0B60CEBA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4152900" y="8382000"/>
+          <a:ext cx="10410825" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.40385</cdr:x>
+      <cdr:y>0.93862</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.48776</cdr:x>
+      <cdr:y>0.98977</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="CaixaDeTexto 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F8B6271-51FA-4FDC-9417-6429B16278F1}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="4400550" y="5243513"/>
+          <a:ext cx="914400" cy="285749"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Popularidade</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Caio" refreshedDate="43368.037623263888" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="190">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Caio" refreshedDate="43368.037623263888" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="190" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabela1"/>
   </cacheSource>
@@ -5853,7 +6939,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Caio" refreshedDate="43427.43493333333" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="190">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Caio" refreshedDate="43427.43493333333" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="190" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabela13"/>
   </cacheSource>
@@ -9717,782 +10803,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="B20:C32" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField name="Repositórios" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="10">
-        <item x="9"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" measureFilter="1" sortType="descending" defaultSubtotal="0">
-      <items count="68">
-        <item x="33"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="34"/>
-        <item x="23"/>
-        <item x="36"/>
-        <item x="30"/>
-        <item x="54"/>
-        <item x="46"/>
-        <item x="28"/>
-        <item x="10"/>
-        <item x="50"/>
-        <item x="67"/>
-        <item x="13"/>
-        <item x="25"/>
-        <item x="6"/>
-        <item x="62"/>
-        <item x="20"/>
-        <item x="41"/>
-        <item x="52"/>
-        <item x="29"/>
-        <item x="58"/>
-        <item x="4"/>
-        <item x="18"/>
-        <item x="44"/>
-        <item x="38"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="59"/>
-        <item x="43"/>
-        <item x="31"/>
-        <item x="27"/>
-        <item x="65"/>
-        <item x="19"/>
-        <item x="1"/>
-        <item x="48"/>
-        <item x="45"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="14"/>
-        <item x="49"/>
-        <item x="53"/>
-        <item x="17"/>
-        <item x="42"/>
-        <item x="32"/>
-        <item x="60"/>
-        <item x="16"/>
-        <item x="63"/>
-        <item x="55"/>
-        <item x="51"/>
-        <item x="57"/>
-        <item x="56"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="66"/>
-        <item x="64"/>
-        <item x="47"/>
-        <item x="22"/>
-        <item x="24"/>
-        <item x="0"/>
-        <item x="21"/>
-        <item x="37"/>
-        <item x="61"/>
-        <item x="35"/>
-        <item x="26"/>
-        <item x="8"/>
-        <item x="15"/>
-        <item x="5"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="10" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Soma de Cobertura de Documentação" fld="7" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <formats count="8">
-    <format dxfId="36">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="35">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="34">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="33">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="32">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="30">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="29">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="2">
-    <chartFormat chart="1" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="1">
-    <filter fld="2" type="valueGreaterThan" evalOrder="-1" id="1" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters>
-            <customFilter operator="greaterThan" val="0.2"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-  </filters>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="B3:G15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField name="Repositórios" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="10">
-        <item x="9"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="10" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-  </colItems>
-  <dataFields count="5">
-    <dataField name="Arquivos" fld="1" baseField="0" baseItem="0"/>
-    <dataField name="Linguagens" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Linhas Comentadas" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Linhas de Código" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Cobertura de Doc." fld="7" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica16" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="B60:C72" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField name="Repositórios" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="10">
-        <item x="9"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" measureFilter="1" sortType="descending" defaultSubtotal="0">
-      <items count="68">
-        <item x="33"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="34"/>
-        <item x="23"/>
-        <item x="36"/>
-        <item x="30"/>
-        <item x="54"/>
-        <item x="46"/>
-        <item x="28"/>
-        <item x="10"/>
-        <item x="50"/>
-        <item x="67"/>
-        <item x="13"/>
-        <item x="25"/>
-        <item x="6"/>
-        <item x="62"/>
-        <item x="20"/>
-        <item x="41"/>
-        <item x="52"/>
-        <item x="29"/>
-        <item x="58"/>
-        <item x="4"/>
-        <item x="18"/>
-        <item x="44"/>
-        <item x="38"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="59"/>
-        <item x="43"/>
-        <item x="31"/>
-        <item x="27"/>
-        <item x="65"/>
-        <item x="19"/>
-        <item x="1"/>
-        <item x="48"/>
-        <item x="45"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="14"/>
-        <item x="49"/>
-        <item x="53"/>
-        <item x="17"/>
-        <item x="42"/>
-        <item x="32"/>
-        <item x="60"/>
-        <item x="16"/>
-        <item x="63"/>
-        <item x="55"/>
-        <item x="51"/>
-        <item x="57"/>
-        <item x="56"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="66"/>
-        <item x="64"/>
-        <item x="47"/>
-        <item x="22"/>
-        <item x="24"/>
-        <item x="0"/>
-        <item x="21"/>
-        <item x="37"/>
-        <item x="61"/>
-        <item x="35"/>
-        <item x="26"/>
-        <item x="8"/>
-        <item x="15"/>
-        <item x="5"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="10" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Soma de Cobertura de Documentação" fld="7" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <formats count="8">
-    <format dxfId="44">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="43">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="42">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="41">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="40">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="39">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="38">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="37">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="13">
-    <chartFormat chart="1" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="12" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="16">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="17">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="18">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="19">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="1">
-    <filter fld="2" type="valueGreaterThan" evalOrder="-1" id="1" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters>
-            <customFilter operator="greaterThan" val="0.2"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-  </filters>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000003000000}" name="Tabela dinâmica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="B90:D164" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="8">
     <pivotField name="Repositórios" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
@@ -10847,44 +11158,44 @@
     <dataField name="Soma de Cobertura de Documentação" fld="7" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="52">
+    <format dxfId="33">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="32">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="31">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="30">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="28">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="27">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="26">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0" selected="0"/>
@@ -10946,12 +11257,799 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="Tabela dinâmica14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="B20:C32" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField name="Repositórios" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="10">
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" measureFilter="1" sortType="descending" defaultSubtotal="0">
+      <items count="68">
+        <item x="33"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="34"/>
+        <item x="23"/>
+        <item x="36"/>
+        <item x="30"/>
+        <item x="54"/>
+        <item x="46"/>
+        <item x="28"/>
+        <item x="10"/>
+        <item x="50"/>
+        <item x="67"/>
+        <item x="13"/>
+        <item x="25"/>
+        <item x="6"/>
+        <item x="62"/>
+        <item x="20"/>
+        <item x="41"/>
+        <item x="52"/>
+        <item x="29"/>
+        <item x="58"/>
+        <item x="4"/>
+        <item x="18"/>
+        <item x="44"/>
+        <item x="38"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="59"/>
+        <item x="43"/>
+        <item x="31"/>
+        <item x="27"/>
+        <item x="65"/>
+        <item x="19"/>
+        <item x="1"/>
+        <item x="48"/>
+        <item x="45"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="14"/>
+        <item x="49"/>
+        <item x="53"/>
+        <item x="17"/>
+        <item x="42"/>
+        <item x="32"/>
+        <item x="60"/>
+        <item x="16"/>
+        <item x="63"/>
+        <item x="55"/>
+        <item x="51"/>
+        <item x="57"/>
+        <item x="56"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="66"/>
+        <item x="64"/>
+        <item x="47"/>
+        <item x="22"/>
+        <item x="24"/>
+        <item x="0"/>
+        <item x="21"/>
+        <item x="37"/>
+        <item x="61"/>
+        <item x="35"/>
+        <item x="26"/>
+        <item x="8"/>
+        <item x="15"/>
+        <item x="5"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="10" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Soma de Cobertura de Documentação" fld="7" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <formats count="8">
+    <format dxfId="41">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="40">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="39">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="38">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="37">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="35">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="2">
+    <chartFormat chart="1" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="2" type="valueGreaterThan" evalOrder="-1" id="1" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter operator="greaterThan" val="0.2"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="B3:G15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField name="Repositórios" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="10">
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="10" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <dataFields count="5">
+    <dataField name="Arquivos" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Linguagens" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Linhas Comentadas" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Linhas de Código" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Cobertura de Doc." fld="7" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="Tabela dinâmica16" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="B60:C72" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField name="Repositórios" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="10">
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" measureFilter="1" sortType="descending" defaultSubtotal="0">
+      <items count="68">
+        <item x="33"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="34"/>
+        <item x="23"/>
+        <item x="36"/>
+        <item x="30"/>
+        <item x="54"/>
+        <item x="46"/>
+        <item x="28"/>
+        <item x="10"/>
+        <item x="50"/>
+        <item x="67"/>
+        <item x="13"/>
+        <item x="25"/>
+        <item x="6"/>
+        <item x="62"/>
+        <item x="20"/>
+        <item x="41"/>
+        <item x="52"/>
+        <item x="29"/>
+        <item x="58"/>
+        <item x="4"/>
+        <item x="18"/>
+        <item x="44"/>
+        <item x="38"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="59"/>
+        <item x="43"/>
+        <item x="31"/>
+        <item x="27"/>
+        <item x="65"/>
+        <item x="19"/>
+        <item x="1"/>
+        <item x="48"/>
+        <item x="45"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="14"/>
+        <item x="49"/>
+        <item x="53"/>
+        <item x="17"/>
+        <item x="42"/>
+        <item x="32"/>
+        <item x="60"/>
+        <item x="16"/>
+        <item x="63"/>
+        <item x="55"/>
+        <item x="51"/>
+        <item x="57"/>
+        <item x="56"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="66"/>
+        <item x="64"/>
+        <item x="47"/>
+        <item x="22"/>
+        <item x="24"/>
+        <item x="0"/>
+        <item x="21"/>
+        <item x="37"/>
+        <item x="61"/>
+        <item x="35"/>
+        <item x="26"/>
+        <item x="8"/>
+        <item x="15"/>
+        <item x="5"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="10" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Soma de Cobertura de Documentação" fld="7" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <formats count="8">
+    <format dxfId="49">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="48">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="47">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="46">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="45">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="44">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="43">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="42">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="13">
+    <chartFormat chart="1" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="16">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="19">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="2" type="valueGreaterThan" evalOrder="-1" id="1" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter operator="greaterThan" val="0.2"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="Tabela dinâmica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="H3:O15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField name="Repositorio" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
@@ -11062,7 +12160,7 @@
     <dataField name="Cobertura de Documentacao" fld="9" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="4">
+    <format dxfId="14">
       <pivotArea outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="4" selected="0">
@@ -11075,7 +12173,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="13">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -11090,21 +12188,24 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G191" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="A1:G191"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:G191" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A1:G191" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Repo" dataDxfId="24"/>
-    <tableColumn id="2" name="Arq" dataDxfId="23"/>
-    <tableColumn id="3" name="Language" dataDxfId="22"/>
-    <tableColumn id="4" name="Branco" dataDxfId="21"/>
-    <tableColumn id="5" name="Comentadas" dataDxfId="20"/>
-    <tableColumn id="6" name="Code" dataDxfId="19"/>
-    <tableColumn id="7" name="Cobertura" dataDxfId="18" dataCellStyle="Porcentagem">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Repo" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Arq" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Language" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Branco" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Comentadas" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Code" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cobertura" dataDxfId="15" dataCellStyle="Porcentagem">
       <calculatedColumnFormula>Tabela1[[#This Row],[Comentadas]]/Tabela1[[#This Row],[Code]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11113,22 +12214,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela13" displayName="Tabela13" ref="A1:I191" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
-  <autoFilter ref="A1:I191"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela13" displayName="Tabela13" ref="A1:I191" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I191" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Repo" dataDxfId="13"/>
-    <tableColumn id="2" name="Arq" dataDxfId="12"/>
-    <tableColumn id="3" name="Language" dataDxfId="11"/>
-    <tableColumn id="4" name="Branco" dataDxfId="10"/>
-    <tableColumn id="5" name="Comentadas" dataDxfId="9"/>
-    <tableColumn id="6" name="Code" dataDxfId="8"/>
-    <tableColumn id="7" name="Cobertura" dataDxfId="7" dataCellStyle="Porcentagem">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Repo" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Arq" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Language" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Branco" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Comentadas" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Code" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Cobertura" dataDxfId="2" dataCellStyle="Porcentagem">
       <calculatedColumnFormula>Tabela13[[#This Row],[Comentadas]]/Tabela13[[#This Row],[Code]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Stars" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Stars" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(A2,$L$4:$O$13,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Forks" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Forks" dataDxfId="0">
       <calculatedColumnFormula>VLOOKUP(A2,$L$4:$O$13,4,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11398,7 +12499,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11417,22 +12518,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="H1" s="19" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -11453,14 +12554,14 @@
       <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="22"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="26"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -11481,12 +12582,12 @@
       <c r="F3">
         <v>51258</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="25"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="29"/>
       <c r="P3" t="s">
         <v>84</v>
       </c>
@@ -11510,12 +12611,12 @@
       <c r="F4">
         <v>9978</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="25"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="29"/>
       <c r="P4" t="s">
         <v>76</v>
       </c>
@@ -11539,12 +12640,12 @@
       <c r="F5">
         <v>9469</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="25"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
       <c r="P5" t="s">
         <v>77</v>
       </c>
@@ -11568,12 +12669,12 @@
       <c r="F6">
         <v>786</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="25"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="29"/>
       <c r="P6" t="s">
         <v>78</v>
       </c>
@@ -11597,12 +12698,12 @@
       <c r="F7">
         <v>323</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="25"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="29"/>
       <c r="P7" t="s">
         <v>85</v>
       </c>
@@ -11626,12 +12727,12 @@
       <c r="F8">
         <v>257</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="25"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="29"/>
       <c r="P8" t="s">
         <v>79</v>
       </c>
@@ -11655,12 +12756,12 @@
       <c r="F9">
         <v>224</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="25"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="29"/>
       <c r="P9" t="s">
         <v>80</v>
       </c>
@@ -11684,12 +12785,12 @@
       <c r="F10">
         <v>54</v>
       </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="25"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="29"/>
       <c r="P10" t="s">
         <v>81</v>
       </c>
@@ -11713,12 +12814,12 @@
       <c r="F11">
         <v>21</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="25"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="29"/>
       <c r="P11" t="s">
         <v>82</v>
       </c>
@@ -11742,12 +12843,12 @@
       <c r="F12">
         <v>12</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="25"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="29"/>
       <c r="P12" t="s">
         <v>83</v>
       </c>
@@ -11771,20 +12872,20 @@
       <c r="F13">
         <v>3</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="25"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="29"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="25"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -11802,12 +12903,12 @@
       <c r="F15" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="25"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="29"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -11828,12 +12929,12 @@
       <c r="F16">
         <v>306037</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="25"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="29"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -11854,12 +12955,12 @@
       <c r="F17">
         <v>35450</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="25"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="29"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -11880,12 +12981,12 @@
       <c r="F18">
         <v>19796</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="25"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="29"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -11906,12 +13007,12 @@
       <c r="F19">
         <v>16991</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="25"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="29"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -11932,12 +13033,12 @@
       <c r="F20">
         <v>8004</v>
       </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="25"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="29"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -11958,12 +13059,12 @@
       <c r="F21">
         <v>4590</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="25"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="29"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -11984,12 +13085,12 @@
       <c r="F22">
         <v>3474</v>
       </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="25"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="29"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -12010,12 +13111,12 @@
       <c r="F23">
         <v>2129</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="25"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="29"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -12036,12 +13137,12 @@
       <c r="F24">
         <v>1392</v>
       </c>
-      <c r="H24" s="23"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="25"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="29"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -12062,12 +13163,12 @@
       <c r="F25">
         <v>781</v>
       </c>
-      <c r="H25" s="23"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="25"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="29"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -12088,12 +13189,12 @@
       <c r="F26">
         <v>204</v>
       </c>
-      <c r="H26" s="23"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="25"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="29"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -12114,12 +13215,12 @@
       <c r="F27">
         <v>156</v>
       </c>
-      <c r="H27" s="23"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="25"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="29"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -12140,12 +13241,12 @@
       <c r="F28">
         <v>149</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="25"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="29"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -12166,12 +13267,12 @@
       <c r="F29">
         <v>109</v>
       </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="25"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="29"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -12192,20 +13293,20 @@
       <c r="F30">
         <v>16</v>
       </c>
-      <c r="H30" s="23"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="25"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="29"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H31" s="23"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="25"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="29"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
@@ -12223,12 +13324,12 @@
       <c r="F32" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="23"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="25"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="29"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -12249,12 +13350,12 @@
       <c r="F33">
         <v>543088</v>
       </c>
-      <c r="H33" s="23"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="25"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="29"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -12275,12 +13376,12 @@
       <c r="F34">
         <v>188259</v>
       </c>
-      <c r="H34" s="23"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="25"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="29"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -12301,12 +13402,12 @@
       <c r="F35">
         <v>37812</v>
       </c>
-      <c r="H35" s="23"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="25"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="29"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -12327,12 +13428,12 @@
       <c r="F36">
         <v>18229</v>
       </c>
-      <c r="H36" s="23"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="25"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="29"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -12353,12 +13454,12 @@
       <c r="F37">
         <v>13044</v>
       </c>
-      <c r="H37" s="26"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="28"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="32"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -15671,7 +16772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:G164"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -16874,7 +17975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G191"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -21485,11 +22586,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="AD43" sqref="AD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21527,13 +22628,13 @@
       <c r="A2" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="19">
         <v>1331</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="19">
         <v>20326</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="19">
         <v>5135</v>
       </c>
     </row>
@@ -21541,13 +22642,13 @@
       <c r="A3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="19">
         <v>3319</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="19">
         <v>42880</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="19">
         <v>10896</v>
       </c>
       <c r="I3" s="10" t="s">
@@ -21558,13 +22659,13 @@
       <c r="A4" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="19">
         <v>2059</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="19">
         <v>33906</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="19">
         <v>13552</v>
       </c>
       <c r="H4" s="10" t="s">
@@ -21596,34 +22697,34 @@
       <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="19">
         <v>59</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="19">
         <v>842</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="19">
         <v>200</v>
       </c>
       <c r="H5" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="22">
         <v>9067</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="22">
         <v>31</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="22">
         <v>1904537</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="22">
         <v>464010</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="22">
         <v>115103</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="22">
         <v>69923</v>
       </c>
       <c r="O5" s="12">
@@ -21634,34 +22735,34 @@
       <c r="A6" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="19">
         <v>1426</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="19">
         <v>57973</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="19">
         <v>9866</v>
       </c>
       <c r="H6" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="22">
         <v>2938</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="22">
         <v>23</v>
       </c>
-      <c r="K6" s="32">
+      <c r="K6" s="22">
         <v>269578</v>
       </c>
-      <c r="L6" s="32">
+      <c r="L6" s="22">
         <v>58060</v>
       </c>
-      <c r="M6" s="32">
+      <c r="M6" s="22">
         <v>71216</v>
       </c>
-      <c r="N6" s="32">
+      <c r="N6" s="22">
         <v>15949</v>
       </c>
       <c r="O6" s="12">
@@ -21672,34 +22773,34 @@
       <c r="A7" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="19">
         <v>3343</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="19">
         <v>51222</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="19">
         <v>14883</v>
       </c>
       <c r="H7" t="s">
         <v>83</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="22">
         <v>3034</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="22">
         <v>44</v>
       </c>
-      <c r="K7" s="32">
+      <c r="K7" s="22">
         <v>748728</v>
       </c>
-      <c r="L7" s="32">
+      <c r="L7" s="22">
         <v>69814</v>
       </c>
-      <c r="M7" s="32">
+      <c r="M7" s="22">
         <v>64480</v>
       </c>
-      <c r="N7" s="32">
+      <c r="N7" s="22">
         <v>8563</v>
       </c>
       <c r="O7" s="12">
@@ -21710,34 +22811,34 @@
       <c r="A8" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="19">
         <v>41</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="19">
         <v>794</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="19">
         <v>21936</v>
       </c>
       <c r="H8" t="s">
         <v>85</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="22">
         <v>2689</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="22">
         <v>8</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="22">
         <v>149121</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="22">
         <v>394</v>
       </c>
-      <c r="M8" s="32">
+      <c r="M8" s="22">
         <v>57973</v>
       </c>
-      <c r="N8" s="32">
+      <c r="N8" s="22">
         <v>9866</v>
       </c>
       <c r="O8" s="12">
@@ -21748,34 +22849,34 @@
       <c r="A9" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="19">
         <v>3727</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="19">
         <v>71216</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="19">
         <v>15949</v>
       </c>
       <c r="H9" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="22">
         <v>5031</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="22">
         <v>16</v>
       </c>
-      <c r="K9" s="32">
+      <c r="K9" s="22">
         <v>975408</v>
       </c>
-      <c r="L9" s="32">
+      <c r="L9" s="22">
         <v>132313</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="22">
         <v>51222</v>
       </c>
-      <c r="N9" s="32">
+      <c r="N9" s="22">
         <v>14883</v>
       </c>
       <c r="O9" s="12">
@@ -21786,34 +22887,34 @@
       <c r="A10" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="19">
         <v>8854</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="19">
         <v>115103</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="19">
         <v>69923</v>
       </c>
       <c r="H10" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="22">
         <v>5009</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="22">
         <v>15</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="22">
         <v>399278</v>
       </c>
-      <c r="L10" s="32">
+      <c r="L10" s="22">
         <v>69853</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="22">
         <v>42880</v>
       </c>
-      <c r="N10" s="32">
+      <c r="N10" s="22">
         <v>10896</v>
       </c>
       <c r="O10" s="12">
@@ -21824,34 +22925,34 @@
       <c r="A11" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="19">
         <v>2638</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="19">
         <v>64480</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="19">
         <v>8563</v>
       </c>
       <c r="H11" t="s">
         <v>77</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="22">
         <v>7630</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="22">
         <v>19</v>
       </c>
-      <c r="K11" s="32">
+      <c r="K11" s="22">
         <v>822278</v>
       </c>
-      <c r="L11" s="32">
+      <c r="L11" s="22">
         <v>371180</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M11" s="22">
         <v>33906</v>
       </c>
-      <c r="N11" s="32">
+      <c r="N11" s="22">
         <v>13552</v>
       </c>
       <c r="O11" s="12">
@@ -21862,22 +22963,22 @@
       <c r="H12" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="22">
         <v>1192</v>
       </c>
-      <c r="J12" s="32">
+      <c r="J12" s="22">
         <v>11</v>
       </c>
-      <c r="K12" s="32">
+      <c r="K12" s="22">
         <v>72385</v>
       </c>
-      <c r="L12" s="32">
+      <c r="L12" s="22">
         <v>10317</v>
       </c>
-      <c r="M12" s="32">
+      <c r="M12" s="22">
         <v>20326</v>
       </c>
-      <c r="N12" s="32">
+      <c r="N12" s="22">
         <v>5135</v>
       </c>
       <c r="O12" s="12">
@@ -21888,22 +22989,22 @@
       <c r="H13" t="s">
         <v>78</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="22">
         <v>3080</v>
       </c>
-      <c r="J13" s="32">
+      <c r="J13" s="22">
         <v>19</v>
       </c>
-      <c r="K13" s="32">
+      <c r="K13" s="22">
         <v>327424</v>
       </c>
-      <c r="L13" s="32">
+      <c r="L13" s="22">
         <v>33921</v>
       </c>
-      <c r="M13" s="32">
+      <c r="M13" s="22">
         <v>842</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N13" s="22">
         <v>200</v>
       </c>
       <c r="O13" s="12">
@@ -21914,22 +23015,22 @@
       <c r="H14" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="32">
+      <c r="I14" s="22">
         <v>7</v>
       </c>
-      <c r="J14" s="32">
+      <c r="J14" s="22">
         <v>4</v>
       </c>
-      <c r="K14" s="32">
+      <c r="K14" s="22">
         <v>403</v>
       </c>
-      <c r="L14" s="32">
+      <c r="L14" s="22">
         <v>2</v>
       </c>
-      <c r="M14" s="32">
+      <c r="M14" s="22">
         <v>794</v>
       </c>
-      <c r="N14" s="32">
+      <c r="N14" s="22">
         <v>21936</v>
       </c>
       <c r="O14" s="12">
@@ -21952,24 +23053,113 @@
       <c r="L15" s="11">
         <v>1209864</v>
       </c>
-      <c r="M15" s="32">
+      <c r="M15" s="22">
         <v>57141.005263157895</v>
       </c>
-      <c r="N15" s="32">
+      <c r="N15" s="22">
         <v>19985.394736842107</v>
       </c>
       <c r="O15" s="12">
         <v>0.21341226358848078</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0.24363401708656748</v>
+      </c>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="12">
+        <v>0.21537365808782616</v>
+      </c>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" s="12">
+        <v>9.3243474265687937E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>85</v>
+      </c>
+      <c r="I28" s="12">
+        <v>2.6421496636959249E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="12">
+        <v>0.13564887718780244</v>
+      </c>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="12">
+        <v>0.17494828164837531</v>
+      </c>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>77</v>
+      </c>
+      <c r="I31" s="12">
+        <v>0.45140451282899458</v>
+      </c>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>84</v>
+      </c>
+      <c r="I32" s="12">
+        <v>0.14252952959867377</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" s="12">
+        <v>0.10359961395621579</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="12">
+        <v>4.9627791563275434E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22010,10 +23200,10 @@
       <c r="G1" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="21" t="s">
         <v>116</v>
       </c>
     </row>
@@ -22040,11 +23230,11 @@
         <f>Tabela13[[#This Row],[Comentadas]]/Tabela13[[#This Row],[Code]]</f>
         <v>0.19507198876272971</v>
       </c>
-      <c r="H2" s="30">
-        <f t="shared" ref="H2:I33" si="0">VLOOKUP(A2,$L$4:$O$13,3,FALSE)</f>
+      <c r="H2" s="20">
+        <f t="shared" ref="H2:H33" si="0">VLOOKUP(A2,$L$4:$O$13,3,FALSE)</f>
         <v>20326</v>
       </c>
-      <c r="I2" s="30">
+      <c r="I2" s="20">
         <f t="shared" ref="I2:I33" si="1">VLOOKUP(A2,$L$4:$O$13,4,FALSE)</f>
         <v>5135</v>
       </c>
@@ -22127,13 +23317,13 @@
       <c r="L4" t="s">
         <v>84</v>
       </c>
-      <c r="M4" s="29">
+      <c r="M4" s="19">
         <v>1331</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="19">
         <v>20326</v>
       </c>
-      <c r="O4" s="29">
+      <c r="O4" s="19">
         <v>5135</v>
       </c>
     </row>
@@ -22171,13 +23361,13 @@
       <c r="L5" t="s">
         <v>76</v>
       </c>
-      <c r="M5" s="29">
+      <c r="M5" s="19">
         <v>3319</v>
       </c>
-      <c r="N5" s="29">
+      <c r="N5" s="19">
         <v>42880</v>
       </c>
-      <c r="O5" s="29">
+      <c r="O5" s="19">
         <v>10896</v>
       </c>
     </row>
@@ -22215,13 +23405,13 @@
       <c r="L6" t="s">
         <v>77</v>
       </c>
-      <c r="M6" s="29">
+      <c r="M6" s="19">
         <v>2059</v>
       </c>
-      <c r="N6" s="29">
+      <c r="N6" s="19">
         <v>33906</v>
       </c>
-      <c r="O6" s="29">
+      <c r="O6" s="19">
         <v>13552</v>
       </c>
     </row>
@@ -22259,13 +23449,13 @@
       <c r="L7" t="s">
         <v>78</v>
       </c>
-      <c r="M7" s="29">
+      <c r="M7" s="19">
         <v>59</v>
       </c>
-      <c r="N7" s="29">
+      <c r="N7" s="19">
         <v>842</v>
       </c>
-      <c r="O7" s="29">
+      <c r="O7" s="19">
         <v>200</v>
       </c>
     </row>
@@ -22303,13 +23493,13 @@
       <c r="L8" t="s">
         <v>85</v>
       </c>
-      <c r="M8" s="29">
+      <c r="M8" s="19">
         <v>1426</v>
       </c>
-      <c r="N8" s="29">
+      <c r="N8" s="19">
         <v>57973</v>
       </c>
-      <c r="O8" s="29">
+      <c r="O8" s="19">
         <v>9866</v>
       </c>
     </row>
@@ -22347,13 +23537,13 @@
       <c r="L9" t="s">
         <v>79</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9" s="19">
         <v>3343</v>
       </c>
-      <c r="N9" s="29">
+      <c r="N9" s="19">
         <v>51222</v>
       </c>
-      <c r="O9" s="29">
+      <c r="O9" s="19">
         <v>14883</v>
       </c>
     </row>
@@ -22391,13 +23581,13 @@
       <c r="L10" t="s">
         <v>80</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="19">
         <v>41</v>
       </c>
-      <c r="N10" s="29">
+      <c r="N10" s="19">
         <v>794</v>
       </c>
-      <c r="O10" s="29">
+      <c r="O10" s="19">
         <v>21936</v>
       </c>
     </row>
@@ -22435,13 +23625,13 @@
       <c r="L11" t="s">
         <v>81</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="19">
         <v>3727</v>
       </c>
-      <c r="N11" s="29">
+      <c r="N11" s="19">
         <v>71216</v>
       </c>
-      <c r="O11" s="29">
+      <c r="O11" s="19">
         <v>15949</v>
       </c>
     </row>
@@ -22479,13 +23669,13 @@
       <c r="L12" t="s">
         <v>82</v>
       </c>
-      <c r="M12" s="29">
+      <c r="M12" s="19">
         <v>8854</v>
       </c>
-      <c r="N12" s="29">
+      <c r="N12" s="19">
         <v>115103</v>
       </c>
-      <c r="O12" s="29">
+      <c r="O12" s="19">
         <v>69923</v>
       </c>
     </row>
@@ -22523,13 +23713,13 @@
       <c r="L13" t="s">
         <v>83</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="19">
         <v>2638</v>
       </c>
-      <c r="N13" s="29">
+      <c r="N13" s="19">
         <v>64480</v>
       </c>
-      <c r="O13" s="29">
+      <c r="O13" s="19">
         <v>8563</v>
       </c>
     </row>

</xml_diff>